<commit_message>
feat: Enhance segment split windows documentation and schema updates
</commit_message>
<xml_diff>
--- a/sample_input.xlsx
+++ b/sample_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/np85685/Development/strava/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924C6D0C-8C2F-3941-B103-71F3FAB9C01B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE064844-98F6-5E48-8892-437E083BA553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>2025-08-31T23:59:59Z</t>
+  </si>
+  <si>
+    <t>Minimum Distance (m)</t>
   </si>
 </sst>
 </file>
@@ -276,14 +279,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -292,6 +292,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -643,25 +649,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -669,7 +675,7 @@
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="6">
         <v>100000001</v>
       </c>
       <c r="C2" t="s">
@@ -749,10 +755,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -760,30 +766,34 @@
     <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="19.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1">
+      <c r="A1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -796,14 +806,17 @@
       <c r="D2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="7">
         <v>4.1666666666666657E-2</v>
       </c>
       <c r="F2">
+        <v>1000</v>
+      </c>
+      <c r="G2">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -816,14 +829,17 @@
       <c r="D3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="7">
         <v>2.777777777777778E-2</v>
       </c>
       <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -836,14 +852,17 @@
       <c r="D4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="7">
         <v>4.1666666666666657E-2</v>
       </c>
       <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -856,14 +875,17 @@
       <c r="D5" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="7">
         <v>4.1666666666666657E-2</v>
       </c>
       <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -876,14 +898,17 @@
       <c r="D6" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="7">
         <v>2.4305555555555559E-2</v>
       </c>
       <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -896,14 +921,17 @@
       <c r="D7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="7">
         <v>4.1666666666666657E-2</v>
       </c>
       <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -916,10 +944,13 @@
       <c r="D8" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="7">
         <v>4.1666666666666657E-2</v>
       </c>
       <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
         <v>20</v>
       </c>
     </row>
@@ -943,13 +974,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
chore: Update sample input Excel file
</commit_message>
<xml_diff>
--- a/sample_input.xlsx
+++ b/sample_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/np85685/Development/strava/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE064844-98F6-5E48-8892-437E083BA553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401D9B70-3BA1-9248-BA6C-3887C140694F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16480" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Runners" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -114,51 +114,12 @@
     <t>Sandy Slog</t>
   </si>
   <si>
-    <t>2025-04-21T00:00:00Z</t>
-  </si>
-  <si>
-    <t>2025-05-05T00:00:00Z</t>
-  </si>
-  <si>
     <t>Fiveways to Hell</t>
   </si>
   <si>
-    <t>2025-06-01T00:00:00Z</t>
-  </si>
-  <si>
     <t>It's a ball that comes out a cannon</t>
   </si>
   <si>
-    <t>2025-06-16T00:00:00Z</t>
-  </si>
-  <si>
-    <t>Sword in the stepping stone</t>
-  </si>
-  <si>
-    <t>2025-07-14T00:00:00Z</t>
-  </si>
-  <si>
-    <t>Chad Special</t>
-  </si>
-  <si>
-    <t>2025-08-11T00:00:00Z</t>
-  </si>
-  <si>
-    <t>Witches Ladder of Death</t>
-  </si>
-  <si>
-    <t>2025-08-25T00:00:00Z</t>
-  </si>
-  <si>
-    <t>Log Race</t>
-  </si>
-  <si>
-    <t>2025-08-30T06:00:00Z</t>
-  </si>
-  <si>
-    <t>2025-08-30T10:00:00Z</t>
-  </si>
-  <si>
     <t>Distance Threshold (km)</t>
   </si>
   <si>
@@ -175,6 +136,36 @@
   </si>
   <si>
     <t>Minimum Distance (m)</t>
+  </si>
+  <si>
+    <t>Window Label</t>
+  </si>
+  <si>
+    <t>Final Push</t>
+  </si>
+  <si>
+    <t>2026-01-05T00:00:00Z</t>
+  </si>
+  <si>
+    <t>2026-01-12T00:00:00Z</t>
+  </si>
+  <si>
+    <t>2026-01-19T00:00:00Z</t>
+  </si>
+  <si>
+    <t>2026-01-11T23:59:59Z</t>
+  </si>
+  <si>
+    <t>2026-01-18T23:59:59Z</t>
+  </si>
+  <si>
+    <t>2026-01-25T23:59:59Z</t>
+  </si>
+  <si>
+    <t>2026-01-26T00:00:00Z</t>
+  </si>
+  <si>
+    <t>2026-02-01T23:59:59Z</t>
   </si>
 </sst>
 </file>
@@ -634,7 +625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -755,10 +746,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -766,11 +757,12 @@
     <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="19.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5" style="2" customWidth="1"/>
+    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="8" t="s">
         <v>23</v>
       </c>
@@ -784,16 +776,19 @@
         <v>26</v>
       </c>
       <c r="E1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -801,157 +796,144 @@
         <v>28881526</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="7">
+        <v>4.1666666666666657E-2</v>
+      </c>
+      <c r="G2">
+        <v>3500</v>
+      </c>
+      <c r="H2">
         <v>30</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="7">
-        <v>4.1666666666666657E-2</v>
-      </c>
-      <c r="F2">
-        <v>1000</v>
-      </c>
-      <c r="G2">
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>32</v>
       </c>
       <c r="B3">
         <v>38987500</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="7">
+        <v>2.777777777777778E-2</v>
+      </c>
+      <c r="G3">
+        <v>3500</v>
+      </c>
+      <c r="H3">
         <v>30</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="7">
-        <v>2.777777777777778E-2</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B4">
         <v>38955187</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="7">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G4">
+        <v>3500</v>
+      </c>
+      <c r="H4">
         <v>30</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="7">
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5">
+        <v>28881526</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="7">
         <v>4.1666666666666657E-2</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5">
-        <v>25947126</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="G5">
+        <v>3500</v>
+      </c>
+      <c r="H5">
         <v>30</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="7">
-        <v>4.1666666666666657E-2</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>38</v>
-      </c>
       <c r="B6">
-        <v>39649743</v>
+        <v>38987500</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="7">
+        <v>2.777777777777778E-2</v>
+      </c>
+      <c r="G6">
+        <v>3500</v>
+      </c>
+      <c r="H6">
         <v>30</v>
       </c>
-      <c r="D6" s="3" t="s">
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7">
+        <v>38955187</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="7">
-        <v>2.4305555555555559E-2</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7">
-        <v>28443143</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="F7" s="7">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="G7">
+        <v>3500</v>
+      </c>
+      <c r="H7">
         <v>30</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="7">
-        <v>4.1666666666666657E-2</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8">
-        <v>34900097</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="7">
-        <v>4.1666666666666657E-2</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -981,15 +963,15 @@
         <v>26</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C2">
         <v>50</v>
@@ -997,10 +979,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C3">
         <v>50</v>
@@ -1008,10 +990,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C4">
         <v>50</v>

</xml_diff>

<commit_message>
chore: Update sample_input.xlsx with new data
</commit_message>
<xml_diff>
--- a/sample_input.xlsx
+++ b/sample_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/np85685/Development/strava/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401D9B70-3BA1-9248-BA6C-3887C140694F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90798103-306A-7F49-BD12-FEF98E9F58D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16480" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21780" yWindow="-20940" windowWidth="38100" windowHeight="20800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Runners" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>2026-02-01T23:59:59Z</t>
+  </si>
+  <si>
+    <t>Time Bonus (secs)</t>
   </si>
 </sst>
 </file>
@@ -625,7 +628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -746,10 +749,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -760,9 +763,10 @@
     <col min="5" max="5" width="19.5" style="2" customWidth="1"/>
     <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="8" t="s">
         <v>23</v>
       </c>
@@ -787,8 +791,11 @@
       <c r="H1" s="8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -811,7 +818,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -833,8 +840,11 @@
       <c r="H3">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -857,8 +867,11 @@
       <c r="H4">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -884,7 +897,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -910,7 +923,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>31</v>
       </c>

</xml_diff>